<commit_message>
Major progress has been made to make tabs for several machine setups
</commit_message>
<xml_diff>
--- a/TPV_Source/test.xlsx
+++ b/TPV_Source/test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Spindel</t>
   </si>
@@ -62,6 +62,9 @@
   <si>
     <t xml:space="preserve">
 </t>
+  </si>
+  <si>
+    <t>16.04.2018, Mon</t>
   </si>
 </sst>
 </file>
@@ -703,7 +706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,6 +793,41 @@
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added popup info when there is a problem with the app config
</commit_message>
<xml_diff>
--- a/TPV_Source/test.xlsx
+++ b/TPV_Source/test.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12225" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="January" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,12 +21,12 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="December" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Spindel</t>
   </si>
@@ -57,14 +58,7 @@
     <t>Annet:</t>
   </si>
   <si>
-    <t>07.04.2018, Sat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
-    <t>16.04.2018, Mon</t>
+    <t>17.04.2018, Tue</t>
   </si>
 </sst>
 </file>
@@ -105,7 +99,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -406,7 +400,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -457,7 +451,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -508,7 +502,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -559,7 +553,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -610,7 +604,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -661,7 +655,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -706,126 +700,76 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="13.85546875"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="7.7109375"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="15.7109375"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="15.85546875"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="16.28515625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="20.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="15.85546875"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="15.28515625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" width="15.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" t="s">
-        <v>11</v>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +789,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -896,7 +840,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -947,7 +891,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -998,7 +942,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
@@ -1049,7 +993,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
we got the colors moving
</commit_message>
<xml_diff>
--- a/TPV_Source/test.xlsx
+++ b/TPV_Source/test.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Spindel</t>
   </si>
@@ -63,6 +63,9 @@
   <si>
     <t xml:space="preserve">
 </t>
+  </si>
+  <si>
+    <t>15.05.2018, Tue</t>
   </si>
 </sst>
 </file>
@@ -755,7 +758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -830,6 +833,41 @@
         <v>11</v>
       </c>
     </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
removed use of deprecated methods in openpyxl
</commit_message>
<xml_diff>
--- a/TPV_Source/test.xlsx
+++ b/TPV_Source/test.xlsx
@@ -58,7 +58,7 @@
     <t>Annet:</t>
   </si>
   <si>
-    <t>01.06.2018, Fri</t>
+    <t>02.06.2018, Sat</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -806,78 +806,78 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made label coloring for weekly persistant even if you dont run the application on relevant days
</commit_message>
<xml_diff>
--- a/TPV_Source/test.xlsx
+++ b/TPV_Source/test.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="8" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12465" windowWidth="20775" xWindow="270" yWindow="600"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="January" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,12 +20,12 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="December" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Spindel</t>
   </si>
@@ -58,14 +57,11 @@
     <t>Annet:</t>
   </si>
   <si>
-    <t>03.09.2018, Mon</t>
+    <t>12.09.2018, Wed</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
-  </si>
-  <si>
-    <t>10.09.2018, Mon</t>
   </si>
 </sst>
 </file>
@@ -106,7 +102,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -962,116 +958,89 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
added yearly and some date magic
</commit_message>
<xml_diff>
--- a/TPV_Source/test.xlsx
+++ b/TPV_Source/test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Spindel</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>17.09.2018, Mon</t>
+  </si>
+  <si>
+    <t>19.09.2018, Wed</t>
   </si>
 </sst>
 </file>
@@ -964,7 +967,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
@@ -1112,6 +1115,41 @@
         <v>11</v>
       </c>
     </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
movable dates method refined
</commit_message>
<xml_diff>
--- a/TPV_Source/test.xlsx
+++ b/TPV_Source/test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Spindel</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>19.09.2018, Wed</t>
+  </si>
+  <si>
+    <t>21.09.2018, Fri</t>
   </si>
 </sst>
 </file>
@@ -967,7 +970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
@@ -1050,7 +1053,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11"/>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>12</v>
@@ -1147,6 +1149,41 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>